<commit_message>
add tests for email/sms solutions
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway\UpNorway_DDF\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A68576-BAA4-477F-B240-CDFAD6D287C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6820927-B0A0-4EC5-9D8E-B52BCA0EFDE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="SendEnquiry" sheetId="4" r:id="rId3"/>
     <sheet name="SearchAnything" sheetId="6" r:id="rId4"/>
     <sheet name="routing" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
-    <sheet name="TailorMyJourney" sheetId="5" r:id="rId7"/>
+    <sheet name="loginToForest" sheetId="9" r:id="rId6"/>
+    <sheet name="email_solution" sheetId="7" r:id="rId7"/>
+    <sheet name="TailorMyJourney" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>firstname</t>
   </si>
@@ -196,6 +197,45 @@
   </si>
   <si>
     <t>http://upnorway.com/journey/the-discovery-route</t>
+  </si>
+  <si>
+    <t>shortlink</t>
+  </si>
+  <si>
+    <t>forestlink</t>
+  </si>
+  <si>
+    <t>https://admin.upnorway.com/39039/data/1571794/index/record/1571792/561/summary</t>
+  </si>
+  <si>
+    <t>https://qa.upnorway.net/partner-experience-confirmation/e5af5490-daa6-11e9-9c60-6faa94e82755/message</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>auto first message</t>
+  </si>
+  <si>
+    <t>auto first reply</t>
+  </si>
+  <si>
+    <t>auto third message</t>
+  </si>
+  <si>
+    <t>auto third reply</t>
+  </si>
+  <si>
+    <t>https://admin.upnorway.com/39039/data/1571794/index/record/1571792/537/summary</t>
+  </si>
+  <si>
+    <t>https://qa.upnorway.net/partner-experience-confirmation/21ae5b60-c7df-11e9-8a1b-5da771ba9daa/message</t>
+  </si>
+  <si>
+    <t>arshad first message</t>
+  </si>
+  <si>
+    <t>arshad second reply 888</t>
   </si>
 </sst>
 </file>
@@ -240,10 +280,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D52AD3C-B256-42A8-80DD-419B790CC7E2}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -848,18 +894,136 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC5E324-C074-4332-9D45-2242E795D187}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EB53FE2F-FCE7-4D92-AD9C-2F897978EA08}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="3" customWidth="1"/>
+    <col min="2" max="3" width="34.44140625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{56FC9715-D3CE-440C-B606-113EFA0ACA1B}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{50DD216D-8864-42B1-BC57-807FB8BF3321}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{8A59FD08-5753-4B89-9A0D-BE9F61B481DF}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{B5CA4474-FC79-43D7-9C92-0FBF326FA52A}"/>
+    <hyperlink ref="A3" r:id="rId5" xr:uid="{2CAD96D2-B8C6-4FDC-8DAE-E2638C7B1046}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{C9DA61C3-866C-45CA-8C06-62E2DBD0CA49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>

</xml_diff>

<commit_message>
modfied data to suite staging env
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway\UpNorway_DDF\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6820927-B0A0-4EC5-9D8E-B52BCA0EFDE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641020FF-3164-492A-B36F-53AC0EE73FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>firstname</t>
   </si>
@@ -236,13 +236,37 @@
   </si>
   <si>
     <t>arshad second reply 888</t>
+  </si>
+  <si>
+    <t>https://admin.upnorway.com/39042/data/1571867/index/record/1571865/389/summary</t>
+  </si>
+  <si>
+    <t>https://stag.upnorway.net/partner-experience-confirmation/91c1f460-d94c-11e9-ac5b-e3e736247283/message</t>
+  </si>
+  <si>
+    <t>https://admin.upnorway.com/39042/data/1571867/index/record/1571865/393/summary</t>
+  </si>
+  <si>
+    <t>https://stag.upnorway.net/partner-experience-confirmation/72896100-d9d8-11e9-bdb9-ab6150a97012/message</t>
+  </si>
+  <si>
+    <t>arshad staging env m1</t>
+  </si>
+  <si>
+    <t>arshad stag evn reply 1</t>
+  </si>
+  <si>
+    <t>scond exp message1</t>
+  </si>
+  <si>
+    <t>second exp reply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,13 +282,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -276,11 +318,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -290,9 +333,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,10 +976,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +1020,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -990,7 +1037,7 @@
         <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1008,6 +1055,40 @@
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1018,8 +1099,13 @@
     <hyperlink ref="B4" r:id="rId4" xr:uid="{B5CA4474-FC79-43D7-9C92-0FBF326FA52A}"/>
     <hyperlink ref="A3" r:id="rId5" xr:uid="{2CAD96D2-B8C6-4FDC-8DAE-E2638C7B1046}"/>
     <hyperlink ref="A4" r:id="rId6" xr:uid="{C9DA61C3-866C-45CA-8C06-62E2DBD0CA49}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{1EB20932-4520-4C4C-B135-167A20F142A2}"/>
+    <hyperlink ref="A5" r:id="rId8" xr:uid="{250F9700-4FBE-4F69-A57D-D0E766CCEC85}"/>
+    <hyperlink ref="B6" r:id="rId9" xr:uid="{60AA705A-A402-41FF-9171-F3573C4F8D20}"/>
+    <hyperlink ref="A6" r:id="rId10" xr:uid="{F56ADDF6-2BF0-4873-BAB2-451BE6F12F68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modified excel to have stag data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway\UpNorway_DDF\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641020FF-3164-492A-B36F-53AC0EE73FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF0F061-3E26-40E7-B5FB-1A0A4219C52F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>firstname</t>
   </si>
@@ -942,19 +942,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC5E324-C074-4332-9D45-2242E795D187}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -962,13 +965,22 @@
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{EB53FE2F-FCE7-4D92-AD9C-2F897978EA08}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3BF0FC1A-B959-4997-8359-6AE20BA6C72F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -978,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
incrased timout for forest admin loading
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway\UpNorway_DDF\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF0F061-3E26-40E7-B5FB-1A0A4219C52F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AE54B1-860C-492B-BE0B-18AF04493FBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="5376" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -944,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC5E324-C074-4332-9D45-2242E795D187}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -990,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>